<commit_message>
Makes inventories load faster
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
@@ -306,12 +306,6 @@
     <t>molybdenum trioxide</t>
   </si>
   <si>
-    <t>market for nickel, 99.5%</t>
-  </si>
-  <si>
-    <t>nickel, 99.5%</t>
-  </si>
-  <si>
     <t>market for portafer</t>
   </si>
   <si>
@@ -368,6 +362,12 @@
   </si>
   <si>
     <t>ton kilometer</t>
+  </si>
+  <si>
+    <t>market for nickel, class 1</t>
+  </si>
+  <si>
+    <t>nickel, class 1</t>
   </si>
 </sst>
 </file>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H759"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +775,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -867,7 +867,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B17">
         <f>250/1000</f>
@@ -978,7 +978,7 @@
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F17" t="s">
         <v>0</v>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -995,7 +995,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1051,7 +1051,7 @@
         <v>42</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1084,7 +1084,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33">
         <f>250/1000</f>
@@ -1189,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F33" t="s">
         <v>0</v>
@@ -1198,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1206,7 +1206,7 @@
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1262,7 +1262,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1295,7 +1295,7 @@
     </row>
     <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B51">
         <f>250/1000</f>
@@ -1444,7 +1444,7 @@
         <v>22</v>
       </c>
       <c r="E51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F51" t="s">
         <v>0</v>
@@ -1453,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1461,7 +1461,7 @@
         <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1517,7 +1517,7 @@
         <v>42</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1550,7 +1550,7 @@
     </row>
     <row r="63" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B69">
         <f>250/1000</f>
@@ -1699,7 +1699,7 @@
         <v>22</v>
       </c>
       <c r="E69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F69" t="s">
         <v>0</v>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2672,7 +2672,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B131">
         <v>1.6910012049805864E-6</v>
@@ -2690,12 +2690,12 @@
         <v>0</v>
       </c>
       <c r="H131" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B132">
         <v>2.6029999999999999E-6</v>
@@ -2713,12 +2713,12 @@
         <v>0</v>
       </c>
       <c r="H132" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B133">
         <v>3.9999999999999998E-7</v>
@@ -2736,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="H133" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -2787,7 +2787,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B136">
         <v>7.35751288389381E-6</v>
@@ -2805,12 +2805,12 @@
         <v>0</v>
       </c>
       <c r="H136" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B137">
         <v>3.095E-6</v>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="H137" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
@@ -2856,7 +2856,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B139">
         <v>3.2659798657742239E-2</v>
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
       <c r="H139" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3602,7 +3602,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B174">
         <v>1.7456639888883143E-6</v>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="H174" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
@@ -3694,7 +3694,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B178">
         <v>1.6910012049805864E-6</v>
@@ -3712,12 +3712,12 @@
         <v>0</v>
       </c>
       <c r="H178" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B179">
         <v>2.6029999999999999E-6</v>
@@ -3735,12 +3735,12 @@
         <v>0</v>
       </c>
       <c r="H179" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B180">
         <v>3.9999999999999998E-7</v>
@@ -3758,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="H180" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
@@ -3809,7 +3809,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B183">
         <v>7.35751288389381E-6</v>
@@ -3827,12 +3827,12 @@
         <v>0</v>
       </c>
       <c r="H183" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B184">
         <v>3.095E-6</v>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="H184" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
@@ -3878,7 +3878,7 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B186">
         <v>3.2105382134671748E-2</v>
@@ -3896,7 +3896,7 @@
         <v>0</v>
       </c>
       <c r="H186" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4229,7 +4229,7 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B206">
         <v>1.6910012049805864E-6</v>
@@ -4247,12 +4247,12 @@
         <v>0</v>
       </c>
       <c r="H206" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B207">
         <v>2.6029999999999999E-6</v>
@@ -4270,12 +4270,12 @@
         <v>0</v>
       </c>
       <c r="H207" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B208">
         <v>3.9999999999999998E-7</v>
@@ -4293,7 +4293,7 @@
         <v>0</v>
       </c>
       <c r="H208" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
@@ -4344,7 +4344,7 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B211">
         <v>7.35751288389381E-6</v>
@@ -4362,12 +4362,12 @@
         <v>0</v>
       </c>
       <c r="H211" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B212">
         <v>3.095E-6</v>
@@ -4385,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="H212" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
@@ -4413,7 +4413,7 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B214">
         <v>3.2671074618388279E-2</v>
@@ -4431,7 +4431,7 @@
         <v>0</v>
       </c>
       <c r="H214" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="215" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4722,7 +4722,7 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B232">
         <v>2.3642079843686714E-6</v>
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="H232" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
@@ -4814,7 +4814,7 @@
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B236">
         <v>1.6910012049805864E-6</v>
@@ -4832,12 +4832,12 @@
         <v>0</v>
       </c>
       <c r="H236" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B237">
         <v>2.6029999999999999E-6</v>
@@ -4855,12 +4855,12 @@
         <v>0</v>
       </c>
       <c r="H237" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B238">
         <v>3.9999999999999998E-7</v>
@@ -4878,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="H238" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
@@ -4929,7 +4929,7 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B241">
         <v>7.35751288389381E-6</v>
@@ -4947,12 +4947,12 @@
         <v>0</v>
       </c>
       <c r="H241" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B242">
         <v>3.095E-6</v>
@@ -4970,7 +4970,7 @@
         <v>0</v>
       </c>
       <c r="H242" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -4998,7 +4998,7 @@
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B244">
         <v>3.267116725616355E-2</v>
@@ -5016,7 +5016,7 @@
         <v>0</v>
       </c>
       <c r="H244" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix CCS input in NG SMR H2 datasets.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5E1256-CDBD-7041-BA93-3BAAA875932D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D665F0-553C-B84D-AE46-B5064C4868D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33340" yWindow="400" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrogen" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
     <t>hydrogen, gaseous, 25 bar</t>
   </si>
   <si>
-    <t>carbon dioxide storage at hydrogen production plant, pre, pipeline 400km, storage 3000m</t>
+    <t>carbon dioxide, captured at hydrogen production plant, pre, pipeline 200km, storage 1000m</t>
   </si>
 </sst>
 </file>
@@ -690,13 +690,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="100.6640625" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add outgoing water flows for the nat gas SMR process.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D665F0-553C-B84D-AE46-B5064C4868D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CA255B-FB2C-8947-AFAC-7B2FEFE1D0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33340" yWindow="400" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrogen" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hydrogen!$A$1:$H$670</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hydrogen!$A$1:$H$676</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="94">
   <si>
     <t>technosphere</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>carbon dioxide, captured at hydrogen production plant, pre, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -688,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H670"/>
+  <dimension ref="A1:H676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2200,62 +2206,56 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B78">
-        <v>6.1611670196058146</v>
+        <v>0.375</v>
       </c>
       <c r="C78" t="s">
-        <v>34</v>
-      </c>
-      <c r="D78" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E78" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F78" t="s">
+        <v>93</v>
       </c>
       <c r="G78" t="s">
-        <v>0</v>
-      </c>
-      <c r="H78" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B79">
-        <v>5.347707144163827E-10</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="C79" t="s">
-        <v>34</v>
-      </c>
-      <c r="D79" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E79" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="F79" t="s">
+        <v>36</v>
       </c>
       <c r="G79" t="s">
-        <v>0</v>
-      </c>
-      <c r="H79" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="B80">
-        <v>5.3272799999999989E-4</v>
+        <v>6.1611670196058146</v>
       </c>
       <c r="C80" t="s">
         <v>34</v>
       </c>
       <c r="D80" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="E80" t="s">
         <v>1</v>
@@ -2264,44 +2264,44 @@
         <v>0</v>
       </c>
       <c r="H80" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B81">
-        <v>3.6000000000000001E-5</v>
+        <v>5.347707144163827E-10</v>
       </c>
       <c r="C81" t="s">
         <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E81" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G81" t="s">
         <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B82">
-        <v>3.6239999999999997E-4</v>
+        <v>5.3272799999999989E-4</v>
       </c>
       <c r="C82" t="s">
         <v>34</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E82" t="s">
         <v>1</v>
@@ -2310,15 +2310,15 @@
         <v>0</v>
       </c>
       <c r="H82" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B83">
-        <v>2.0947967866659771E-4</v>
+        <v>3.6000000000000001E-5</v>
       </c>
       <c r="C83" t="s">
         <v>34</v>
@@ -2333,15 +2333,15 @@
         <v>0</v>
       </c>
       <c r="H83" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B84">
-        <v>2.54628E-9</v>
+        <v>3.6239999999999997E-4</v>
       </c>
       <c r="C84" t="s">
         <v>34</v>
@@ -2350,21 +2350,21 @@
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G84" t="s">
         <v>0</v>
       </c>
       <c r="H84" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B85">
-        <v>2.796E-5</v>
+        <v>2.0947967866659771E-4</v>
       </c>
       <c r="C85" t="s">
         <v>34</v>
@@ -2379,15 +2379,15 @@
         <v>0</v>
       </c>
       <c r="H85" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B86">
-        <v>1.668E-5</v>
+        <v>2.54628E-9</v>
       </c>
       <c r="C86" t="s">
         <v>34</v>
@@ -2396,21 +2396,21 @@
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G86" t="s">
         <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B87">
-        <v>2.0292014459767036E-4</v>
+        <v>2.796E-5</v>
       </c>
       <c r="C87" t="s">
         <v>34</v>
@@ -2425,15 +2425,15 @@
         <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B88">
-        <v>3.1235999999999997E-4</v>
+        <v>1.668E-5</v>
       </c>
       <c r="C88" t="s">
         <v>34</v>
@@ -2448,21 +2448,21 @@
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B89">
-        <v>4.8000000000000001E-5</v>
+        <v>2.0292014459767036E-4</v>
       </c>
       <c r="C89" t="s">
         <v>34</v>
       </c>
       <c r="D89" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E89" t="s">
         <v>1</v>
@@ -2471,15 +2471,15 @@
         <v>0</v>
       </c>
       <c r="H89" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="B90">
-        <v>1.1591999999999998E-5</v>
+        <v>3.1235999999999997E-4</v>
       </c>
       <c r="C90" t="s">
         <v>34</v>
@@ -2494,21 +2494,21 @@
         <v>0</v>
       </c>
       <c r="H90" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B91">
-        <v>7.5375498599112571</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="C91" t="s">
         <v>34</v>
       </c>
       <c r="D91" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E91" t="s">
         <v>1</v>
@@ -2517,15 +2517,15 @@
         <v>0</v>
       </c>
       <c r="H91" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="B92">
-        <v>8.8290154606725723E-4</v>
+        <v>1.1591999999999998E-5</v>
       </c>
       <c r="C92" t="s">
         <v>34</v>
@@ -2540,21 +2540,21 @@
         <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B93">
-        <v>3.7140000000000003E-4</v>
+        <v>7.5375498599112571</v>
       </c>
       <c r="C93" t="s">
         <v>34</v>
       </c>
       <c r="D93" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E93" t="s">
         <v>1</v>
@@ -2563,335 +2563,329 @@
         <v>0</v>
       </c>
       <c r="H93" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>8.8290154606725723E-4</v>
       </c>
       <c r="C94" t="s">
         <v>34</v>
       </c>
       <c r="D94" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E94" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G94" t="s">
         <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95">
+        <v>3.7140000000000003E-4</v>
+      </c>
+      <c r="C95" t="s">
+        <v>34</v>
+      </c>
+      <c r="D95" t="s">
+        <v>2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>1</v>
+      </c>
+      <c r="G95" t="s">
+        <v>0</v>
+      </c>
+      <c r="H95" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>34</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" t="s">
+        <v>0</v>
+      </c>
+      <c r="H96" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>78</v>
       </c>
-      <c r="B95">
+      <c r="B97">
         <f>(B50*120)/36</f>
         <v>4.3011681308121101</v>
       </c>
-      <c r="C95" t="s">
-        <v>34</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="C97" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" t="s">
         <v>14</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E97" t="s">
         <v>21</v>
       </c>
-      <c r="G95" t="s">
-        <v>0</v>
-      </c>
-      <c r="H95" t="s">
+      <c r="G97" t="s">
+        <v>0</v>
+      </c>
+      <c r="H97" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>33</v>
-      </c>
-      <c r="B98">
-        <v>1.3068429847355314</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>7</v>
-      </c>
-      <c r="B99" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>5</v>
-      </c>
-      <c r="B100" t="s">
-        <v>90</v>
+        <v>33</v>
+      </c>
+      <c r="B100">
+        <v>1.3068429847355314</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>11</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" t="s">
-        <v>8</v>
-      </c>
-      <c r="D104" t="s">
-        <v>7</v>
-      </c>
-      <c r="E104" t="s">
-        <v>4</v>
-      </c>
-      <c r="F104" t="s">
-        <v>23</v>
-      </c>
-      <c r="G104" t="s">
-        <v>6</v>
-      </c>
-      <c r="H104" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" t="str">
-        <f>B97</f>
-        <v>hydrogen production, auto-thermal reforming of natural gas, 25 bar</v>
-      </c>
-      <c r="B105">
-        <v>1</v>
-      </c>
-      <c r="C105" t="s">
-        <v>31</v>
-      </c>
-      <c r="D105" t="s">
-        <v>15</v>
-      </c>
-      <c r="E105" t="s">
-        <v>1</v>
-      </c>
-      <c r="G105" t="s">
-        <v>3</v>
-      </c>
-      <c r="H105" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>28</v>
-      </c>
-      <c r="B106">
-        <v>8.9868381043588528</v>
+        <v>10</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D106" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E106" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F106" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G106" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="H106" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>46</v>
+      <c r="A107" t="str">
+        <f>B99</f>
+        <v>hydrogen production, auto-thermal reforming of natural gas, 25 bar</v>
       </c>
       <c r="B107">
-        <v>2.9996721816189444E-3</v>
+        <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D107" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E107" t="s">
         <v>1</v>
       </c>
-      <c r="F107" t="s">
-        <v>36</v>
-      </c>
       <c r="G107" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="H107" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B108">
-        <v>0.38041197561668283</v>
+        <v>8.9868381043588528</v>
       </c>
       <c r="C108" t="s">
         <v>27</v>
       </c>
+      <c r="D108" t="s">
+        <v>29</v>
+      </c>
       <c r="E108" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G108" t="s">
         <v>26</v>
+      </c>
+      <c r="H108" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B109">
-        <v>5.3487471618165237E-10</v>
+        <v>2.9996721816189444E-3</v>
       </c>
       <c r="C109" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D109" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E109" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="F109" t="s">
+        <v>36</v>
       </c>
       <c r="G109" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H109" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B110">
-        <v>5.3272799999999989E-4</v>
+        <v>0.38041197561668283</v>
       </c>
       <c r="C110" t="s">
-        <v>34</v>
-      </c>
-      <c r="D110" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E110" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F110" t="s">
+        <v>30</v>
       </c>
       <c r="G110" t="s">
-        <v>0</v>
-      </c>
-      <c r="H110" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B111">
-        <v>3.6000000000000001E-5</v>
+        <v>0.375</v>
       </c>
       <c r="C111" t="s">
-        <v>34</v>
-      </c>
-      <c r="D111" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E111" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F111" t="s">
+        <v>93</v>
       </c>
       <c r="G111" t="s">
-        <v>0</v>
-      </c>
-      <c r="H111" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B112">
-        <v>3.6239999999999997E-4</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="C112" t="s">
-        <v>34</v>
-      </c>
-      <c r="D112" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E112" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F112" t="s">
+        <v>36</v>
       </c>
       <c r="G112" t="s">
-        <v>0</v>
-      </c>
-      <c r="H112" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B113">
-        <v>2.54628E-9</v>
+        <v>5.3487471618165237E-10</v>
       </c>
       <c r="C113" t="s">
         <v>34</v>
       </c>
       <c r="D113" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E113" t="s">
         <v>4</v>
@@ -2900,21 +2894,21 @@
         <v>0</v>
       </c>
       <c r="H113" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B114">
-        <v>2.796E-5</v>
+        <v>5.3272799999999989E-4</v>
       </c>
       <c r="C114" t="s">
         <v>34</v>
       </c>
       <c r="D114" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E114" t="s">
         <v>1</v>
@@ -2923,15 +2917,15 @@
         <v>0</v>
       </c>
       <c r="H114" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B115">
-        <v>1.668E-5</v>
+        <v>3.6000000000000001E-5</v>
       </c>
       <c r="C115" t="s">
         <v>34</v>
@@ -2946,15 +2940,15 @@
         <v>0</v>
       </c>
       <c r="H115" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B116">
-        <v>2.0292014459767036E-4</v>
+        <v>3.6239999999999997E-4</v>
       </c>
       <c r="C116" t="s">
         <v>34</v>
@@ -2969,15 +2963,15 @@
         <v>0</v>
       </c>
       <c r="H116" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B117">
-        <v>3.1235999999999997E-4</v>
+        <v>2.54628E-9</v>
       </c>
       <c r="C117" t="s">
         <v>34</v>
@@ -2986,27 +2980,27 @@
         <v>2</v>
       </c>
       <c r="E117" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G117" t="s">
         <v>0</v>
       </c>
       <c r="H117" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B118">
-        <v>4.8000000000000001E-5</v>
+        <v>2.796E-5</v>
       </c>
       <c r="C118" t="s">
         <v>34</v>
       </c>
       <c r="D118" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E118" t="s">
         <v>1</v>
@@ -3015,15 +3009,15 @@
         <v>0</v>
       </c>
       <c r="H118" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="B119">
-        <v>1.1591999999999998E-5</v>
+        <v>1.668E-5</v>
       </c>
       <c r="C119" t="s">
         <v>34</v>
@@ -3038,21 +3032,21 @@
         <v>0</v>
       </c>
       <c r="H119" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B120">
-        <v>7.5390157563601576</v>
+        <v>2.0292014459767036E-4</v>
       </c>
       <c r="C120" t="s">
         <v>34</v>
       </c>
       <c r="D120" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E120" t="s">
         <v>1</v>
@@ -3061,15 +3055,15 @@
         <v>0</v>
       </c>
       <c r="H120" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B121">
-        <v>8.8290154606725723E-4</v>
+        <v>3.1235999999999997E-4</v>
       </c>
       <c r="C121" t="s">
         <v>34</v>
@@ -3084,21 +3078,21 @@
         <v>0</v>
       </c>
       <c r="H121" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B122">
-        <v>3.7140000000000003E-4</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="C122" t="s">
         <v>34</v>
       </c>
       <c r="D122" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E122" t="s">
         <v>1</v>
@@ -3107,39 +3101,38 @@
         <v>0</v>
       </c>
       <c r="H122" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B123">
-        <v>0</v>
+        <v>1.1591999999999998E-5</v>
       </c>
       <c r="C123" t="s">
         <v>34</v>
       </c>
       <c r="D123" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E123" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G123" t="s">
         <v>0</v>
       </c>
       <c r="H123" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B124">
-        <f>(B98*120)/36</f>
-        <v>4.3561432824517716</v>
+        <v>7.5390157563601576</v>
       </c>
       <c r="C124" t="s">
         <v>34</v>
@@ -3148,203 +3141,201 @@
         <v>14</v>
       </c>
       <c r="E124" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G124" t="s">
         <v>0</v>
       </c>
       <c r="H124" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="2"/>
-      <c r="G125" s="2"/>
-    </row>
-    <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>87</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>74</v>
+      </c>
+      <c r="B125">
+        <v>8.8290154606725723E-4</v>
+      </c>
+      <c r="C125" t="s">
+        <v>34</v>
+      </c>
+      <c r="D125" t="s">
+        <v>2</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1</v>
+      </c>
+      <c r="G125" t="s">
+        <v>0</v>
+      </c>
+      <c r="H125" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>76</v>
+      </c>
+      <c r="B126">
+        <v>3.7140000000000003E-4</v>
+      </c>
+      <c r="C126" t="s">
+        <v>34</v>
+      </c>
+      <c r="D126" t="s">
+        <v>2</v>
+      </c>
+      <c r="E126" t="s">
+        <v>1</v>
+      </c>
+      <c r="G126" t="s">
+        <v>0</v>
+      </c>
+      <c r="H126" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B127">
-        <v>1.3068466902465423</v>
+        <v>0</v>
+      </c>
+      <c r="C127" t="s">
+        <v>34</v>
+      </c>
+      <c r="D127" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" t="s">
+        <v>0</v>
+      </c>
+      <c r="H127" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>7</v>
-      </c>
-      <c r="B128" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>5</v>
-      </c>
-      <c r="B129" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>4</v>
-      </c>
-      <c r="B130" t="s">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B128">
+        <f>(B100*120)/36</f>
+        <v>4.3561432824517716</v>
+      </c>
+      <c r="C128" t="s">
+        <v>34</v>
+      </c>
+      <c r="D128" t="s">
+        <v>14</v>
+      </c>
+      <c r="E128" t="s">
+        <v>21</v>
+      </c>
+      <c r="G128" t="s">
+        <v>0</v>
+      </c>
+      <c r="H128" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="2"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>88</v>
-      </c>
-      <c r="B131" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="B131">
+        <v>1.3068466902465423</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B133" t="s">
-        <v>9</v>
-      </c>
-      <c r="C133" t="s">
-        <v>8</v>
-      </c>
-      <c r="D133" t="s">
-        <v>7</v>
-      </c>
-      <c r="E133" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>4</v>
       </c>
-      <c r="F133" t="s">
-        <v>23</v>
-      </c>
-      <c r="G133" t="s">
-        <v>6</v>
-      </c>
-      <c r="H133" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" t="str">
-        <f>B126</f>
-        <v>hydrogen production, auto-thermal reforming of natural gas, with CCS (MDEA, 98% eff.), 25 bar</v>
-      </c>
-      <c r="B134">
-        <v>1</v>
-      </c>
-      <c r="C134" t="s">
-        <v>31</v>
-      </c>
-      <c r="D134" t="s">
-        <v>15</v>
-      </c>
-      <c r="E134" t="s">
-        <v>1</v>
-      </c>
-      <c r="G134" t="s">
-        <v>3</v>
-      </c>
-      <c r="H134" t="s">
-        <v>90</v>
+      <c r="B134" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>28</v>
-      </c>
-      <c r="B135">
-        <v>0.58838389214647391</v>
-      </c>
-      <c r="C135" t="s">
-        <v>27</v>
-      </c>
-      <c r="D135" t="s">
-        <v>29</v>
-      </c>
-      <c r="E135" t="s">
-        <v>1</v>
-      </c>
-      <c r="F135" t="s">
-        <v>36</v>
-      </c>
-      <c r="G135" t="s">
-        <v>26</v>
-      </c>
-      <c r="H135" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>46</v>
-      </c>
-      <c r="B136">
-        <v>2.9996721816189444E-3</v>
-      </c>
-      <c r="C136" t="s">
-        <v>27</v>
-      </c>
-      <c r="D136" t="s">
-        <v>29</v>
-      </c>
-      <c r="E136" t="s">
-        <v>1</v>
-      </c>
-      <c r="F136" t="s">
-        <v>36</v>
-      </c>
-      <c r="G136" t="s">
-        <v>26</v>
-      </c>
-      <c r="H136" t="s">
-        <v>29</v>
+        <v>88</v>
+      </c>
+      <c r="B135" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>54</v>
-      </c>
-      <c r="B137">
-        <v>0.38041305426253447</v>
+        <v>10</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
       </c>
       <c r="C137" t="s">
-        <v>27</v>
+        <v>8</v>
+      </c>
+      <c r="D137" t="s">
+        <v>7</v>
       </c>
       <c r="E137" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F137" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G137" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="H137" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>91</v>
+      <c r="A138" t="str">
+        <f>B130</f>
+        <v>hydrogen production, auto-thermal reforming of natural gas, with CCS (MDEA, 98% eff.), 25 bar</v>
       </c>
       <c r="B138">
-        <v>8.3442634742423714</v>
+        <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D138" t="s">
         <v>15</v>
@@ -3353,185 +3344,182 @@
         <v>1</v>
       </c>
       <c r="G138" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H138" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B139">
-        <v>5.3487623280160849E-10</v>
+        <v>0.58838389214647391</v>
       </c>
       <c r="C139" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D139" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E139" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="F139" t="s">
+        <v>36</v>
       </c>
       <c r="G139" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H139" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B140">
-        <v>5.3272799999999989E-4</v>
+        <v>2.9996721816189444E-3</v>
       </c>
       <c r="C140" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D140" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E140" t="s">
         <v>1</v>
       </c>
+      <c r="F140" t="s">
+        <v>36</v>
+      </c>
       <c r="G140" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H140" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B141">
-        <v>3.6000000000000001E-5</v>
+        <v>0.38041305426253447</v>
       </c>
       <c r="C141" t="s">
-        <v>34</v>
-      </c>
-      <c r="D141" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E141" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F141" t="s">
+        <v>30</v>
       </c>
       <c r="G141" t="s">
-        <v>0</v>
-      </c>
-      <c r="H141" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B142">
-        <v>3.6239999999999997E-4</v>
+        <v>0.375</v>
       </c>
       <c r="C142" t="s">
-        <v>34</v>
-      </c>
-      <c r="D142" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E142" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F142" t="s">
+        <v>93</v>
       </c>
       <c r="G142" t="s">
-        <v>0</v>
-      </c>
-      <c r="H142" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B143">
-        <v>2.8370495812424056E-4</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="C143" t="s">
-        <v>34</v>
-      </c>
-      <c r="D143" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E143" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F143" t="s">
+        <v>36</v>
       </c>
       <c r="G143" t="s">
-        <v>0</v>
-      </c>
-      <c r="H143" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="B144">
-        <v>2.54628E-9</v>
+        <v>8.3442634742423714</v>
       </c>
       <c r="C144" t="s">
         <v>34</v>
       </c>
       <c r="D144" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E144" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G144" t="s">
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B145">
-        <v>2.796E-5</v>
+        <v>5.3487623280160849E-10</v>
       </c>
       <c r="C145" t="s">
         <v>34</v>
       </c>
       <c r="D145" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E145" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G145" t="s">
         <v>0</v>
       </c>
       <c r="H145" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B146">
-        <v>1.668E-5</v>
+        <v>5.3272799999999989E-4</v>
       </c>
       <c r="C146" t="s">
         <v>34</v>
       </c>
       <c r="D146" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="E146" t="s">
         <v>1</v>
@@ -3540,15 +3528,15 @@
         <v>0</v>
       </c>
       <c r="H146" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B147">
-        <v>2.0292014459767036E-4</v>
+        <v>3.6000000000000001E-5</v>
       </c>
       <c r="C147" t="s">
         <v>34</v>
@@ -3563,15 +3551,15 @@
         <v>0</v>
       </c>
       <c r="H147" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B148">
-        <v>3.1235999999999997E-4</v>
+        <v>3.6239999999999997E-4</v>
       </c>
       <c r="C148" t="s">
         <v>34</v>
@@ -3586,21 +3574,21 @@
         <v>0</v>
       </c>
       <c r="H148" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B149">
-        <v>4.8000000000000001E-5</v>
+        <v>2.8370495812424056E-4</v>
       </c>
       <c r="C149" t="s">
         <v>34</v>
       </c>
       <c r="D149" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E149" t="s">
         <v>1</v>
@@ -3609,15 +3597,15 @@
         <v>0</v>
       </c>
       <c r="H149" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B150">
-        <v>1.1591999999999998E-5</v>
+        <v>2.54628E-9</v>
       </c>
       <c r="C150" t="s">
         <v>34</v>
@@ -3626,27 +3614,27 @@
         <v>2</v>
       </c>
       <c r="E150" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G150" t="s">
         <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="B151">
-        <v>7.5390371329954711</v>
+        <v>2.796E-5</v>
       </c>
       <c r="C151" t="s">
         <v>34</v>
       </c>
       <c r="D151" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E151" t="s">
         <v>1</v>
@@ -3655,15 +3643,15 @@
         <v>0</v>
       </c>
       <c r="H151" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B152">
-        <v>8.8290154606725723E-4</v>
+        <v>1.668E-5</v>
       </c>
       <c r="C152" t="s">
         <v>34</v>
@@ -3678,15 +3666,15 @@
         <v>0</v>
       </c>
       <c r="H152" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B153">
-        <v>3.7140000000000003E-4</v>
+        <v>2.0292014459767036E-4</v>
       </c>
       <c r="C153" t="s">
         <v>34</v>
@@ -3701,326 +3689,464 @@
         <v>0</v>
       </c>
       <c r="H153" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B154">
-        <v>0</v>
+        <v>3.1235999999999997E-4</v>
       </c>
       <c r="C154" t="s">
         <v>34</v>
       </c>
       <c r="D154" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E154" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G154" t="s">
         <v>0</v>
       </c>
       <c r="H154" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>72</v>
+      </c>
+      <c r="B155">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="C155" t="s">
+        <v>34</v>
+      </c>
+      <c r="D155" t="s">
+        <v>15</v>
+      </c>
+      <c r="E155" t="s">
+        <v>1</v>
+      </c>
+      <c r="G155" t="s">
+        <v>0</v>
+      </c>
+      <c r="H155" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>20</v>
+      </c>
+      <c r="B156">
+        <v>1.1591999999999998E-5</v>
+      </c>
+      <c r="C156" t="s">
+        <v>34</v>
+      </c>
+      <c r="D156" t="s">
+        <v>2</v>
+      </c>
+      <c r="E156" t="s">
+        <v>1</v>
+      </c>
+      <c r="G156" t="s">
+        <v>0</v>
+      </c>
+      <c r="H156" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>25</v>
+      </c>
+      <c r="B157">
+        <v>7.5390371329954711</v>
+      </c>
+      <c r="C157" t="s">
+        <v>34</v>
+      </c>
+      <c r="D157" t="s">
+        <v>14</v>
+      </c>
+      <c r="E157" t="s">
+        <v>1</v>
+      </c>
+      <c r="G157" t="s">
+        <v>0</v>
+      </c>
+      <c r="H157" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>74</v>
+      </c>
+      <c r="B158">
+        <v>8.8290154606725723E-4</v>
+      </c>
+      <c r="C158" t="s">
+        <v>34</v>
+      </c>
+      <c r="D158" t="s">
+        <v>2</v>
+      </c>
+      <c r="E158" t="s">
+        <v>1</v>
+      </c>
+      <c r="G158" t="s">
+        <v>0</v>
+      </c>
+      <c r="H158" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>76</v>
+      </c>
+      <c r="B159">
+        <v>3.7140000000000003E-4</v>
+      </c>
+      <c r="C159" t="s">
+        <v>34</v>
+      </c>
+      <c r="D159" t="s">
+        <v>2</v>
+      </c>
+      <c r="E159" t="s">
+        <v>1</v>
+      </c>
+      <c r="G159" t="s">
+        <v>0</v>
+      </c>
+      <c r="H159" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>18</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160" t="s">
+        <v>34</v>
+      </c>
+      <c r="D160" t="s">
+        <v>15</v>
+      </c>
+      <c r="E160" t="s">
+        <v>13</v>
+      </c>
+      <c r="G160" t="s">
+        <v>0</v>
+      </c>
+      <c r="H160" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>78</v>
       </c>
-      <c r="B155">
-        <f>(B127*120)/36</f>
+      <c r="B161">
+        <f>(B131*120)/36</f>
         <v>4.3561556341551411</v>
       </c>
-      <c r="C155" t="s">
-        <v>34</v>
-      </c>
-      <c r="D155" t="s">
+      <c r="C161" t="s">
+        <v>34</v>
+      </c>
+      <c r="D161" t="s">
         <v>14</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E161" t="s">
         <v>21</v>
       </c>
-      <c r="G155" t="s">
-        <v>0</v>
-      </c>
-      <c r="H155" t="s">
+      <c r="G161" t="s">
+        <v>0</v>
+      </c>
+      <c r="H161" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="B156" s="2"/>
-    </row>
-    <row r="160" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="162" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A162" s="2"/>
-      <c r="G162" s="2"/>
-    </row>
-    <row r="171" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
-    </row>
-    <row r="179" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="182" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A182" s="2"/>
-      <c r="G182" s="2"/>
+    <row r="162" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="B162" s="2"/>
+    </row>
+    <row r="166" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="168" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A168" s="2"/>
+      <c r="G168" s="2"/>
+    </row>
+    <row r="177" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+    </row>
+    <row r="185" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A185" s="1"/>
     </row>
     <row r="188" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A188" s="1"/>
-      <c r="B188" s="1"/>
-    </row>
-    <row r="192" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B192" s="2"/>
-    </row>
-    <row r="196" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A196" s="1"/>
+      <c r="A188" s="2"/>
+      <c r="G188" s="2"/>
+    </row>
+    <row r="194" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
     </row>
     <row r="198" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A198" s="2"/>
-      <c r="G198" s="2"/>
-    </row>
-    <row r="207" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A207" s="1"/>
-      <c r="B207" s="1"/>
-    </row>
-    <row r="215" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A215" s="1"/>
-    </row>
-    <row r="218" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A218" s="2"/>
-      <c r="G218" s="2"/>
+      <c r="B198" s="2"/>
+    </row>
+    <row r="202" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A202" s="1"/>
+    </row>
+    <row r="204" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A204" s="2"/>
+      <c r="G204" s="2"/>
+    </row>
+    <row r="213" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
+    </row>
+    <row r="221" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A221" s="1"/>
     </row>
     <row r="224" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A224" s="1"/>
-      <c r="B224" s="1"/>
-    </row>
-    <row r="228" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B228" s="2"/>
-    </row>
-    <row r="232" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A232" s="1"/>
+      <c r="A224" s="2"/>
+      <c r="G224" s="2"/>
+    </row>
+    <row r="230" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A230" s="1"/>
+      <c r="B230" s="1"/>
     </row>
     <row r="234" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A234" s="2"/>
-      <c r="G234" s="2"/>
-    </row>
-    <row r="243" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A243" s="1"/>
-      <c r="B243" s="1"/>
-    </row>
-    <row r="251" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A251" s="1"/>
-    </row>
-    <row r="254" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A254" s="2"/>
-      <c r="G254" s="2"/>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="238" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="240" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A240" s="2"/>
+      <c r="G240" s="2"/>
+    </row>
+    <row r="249" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+    </row>
+    <row r="257" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A257" s="1"/>
     </row>
     <row r="260" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A260" s="1"/>
-      <c r="B260" s="1"/>
-    </row>
-    <row r="264" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B264" s="2"/>
-    </row>
-    <row r="268" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A268" s="1"/>
+      <c r="A260" s="2"/>
+      <c r="G260" s="2"/>
+    </row>
+    <row r="266" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A266" s="1"/>
+      <c r="B266" s="1"/>
     </row>
     <row r="270" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A270" s="2"/>
-      <c r="G270" s="2"/>
-    </row>
-    <row r="279" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A279" s="1"/>
-      <c r="B279" s="1"/>
-    </row>
-    <row r="287" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A287" s="1"/>
-    </row>
-    <row r="290" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A290" s="2"/>
-      <c r="G290" s="2"/>
+      <c r="B270" s="2"/>
+    </row>
+    <row r="274" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A274" s="1"/>
+    </row>
+    <row r="276" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A276" s="2"/>
+      <c r="G276" s="2"/>
+    </row>
+    <row r="285" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A285" s="1"/>
+      <c r="B285" s="1"/>
+    </row>
+    <row r="293" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A293" s="1"/>
     </row>
     <row r="296" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A296" s="1"/>
-      <c r="B296" s="1"/>
-    </row>
-    <row r="300" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B300" s="2"/>
-    </row>
-    <row r="304" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A304" s="1"/>
+      <c r="A296" s="2"/>
+      <c r="G296" s="2"/>
+    </row>
+    <row r="302" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A302" s="1"/>
+      <c r="B302" s="1"/>
     </row>
     <row r="306" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A306" s="2"/>
-      <c r="G306" s="2"/>
-    </row>
-    <row r="315" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A315" s="1"/>
-      <c r="B315" s="1"/>
-    </row>
-    <row r="323" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A323" s="1"/>
-    </row>
-    <row r="326" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A326" s="2"/>
-      <c r="G326" s="2"/>
+      <c r="B306" s="2"/>
+    </row>
+    <row r="310" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A310" s="1"/>
+    </row>
+    <row r="312" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A312" s="2"/>
+      <c r="G312" s="2"/>
+    </row>
+    <row r="321" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A321" s="1"/>
+      <c r="B321" s="1"/>
+    </row>
+    <row r="329" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A329" s="1"/>
     </row>
     <row r="332" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A332" s="1"/>
-      <c r="B332" s="1"/>
-    </row>
-    <row r="336" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B336" s="2"/>
-    </row>
-    <row r="340" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A340" s="1"/>
+      <c r="A332" s="2"/>
+      <c r="G332" s="2"/>
+    </row>
+    <row r="338" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A338" s="1"/>
+      <c r="B338" s="1"/>
     </row>
     <row r="342" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A342" s="2"/>
-      <c r="G342" s="2"/>
-    </row>
-    <row r="351" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A351" s="1"/>
-      <c r="B351" s="1"/>
-    </row>
-    <row r="358" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A358" s="1"/>
-    </row>
-    <row r="369" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A369" s="1"/>
-      <c r="B369" s="1"/>
-    </row>
-    <row r="376" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A376" s="1"/>
-    </row>
-    <row r="387" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A387" s="1"/>
-      <c r="B387" s="1"/>
-    </row>
-    <row r="394" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A394" s="1"/>
-    </row>
-    <row r="406" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A406" s="1"/>
-      <c r="B406" s="1"/>
-    </row>
-    <row r="413" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A413" s="1"/>
-    </row>
-    <row r="428" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A428" s="1"/>
-      <c r="B428" s="1"/>
-    </row>
-    <row r="435" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A435" s="1"/>
-    </row>
-    <row r="440" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A440" s="1"/>
-      <c r="B440" s="1"/>
-    </row>
-    <row r="447" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A447" s="1"/>
-    </row>
-    <row r="455" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A455" s="1"/>
-      <c r="B455" s="1"/>
-    </row>
-    <row r="462" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A462" s="1"/>
-    </row>
-    <row r="471" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A471" s="1"/>
-      <c r="B471" s="1"/>
-    </row>
-    <row r="478" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A478" s="1"/>
-    </row>
-    <row r="485" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A485" s="1"/>
-      <c r="B485" s="1"/>
-    </row>
-    <row r="492" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A492" s="1"/>
-    </row>
-    <row r="505" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A505" s="1"/>
-      <c r="B505" s="1"/>
-    </row>
-    <row r="512" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A512" s="1"/>
-    </row>
-    <row r="522" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A522" s="1"/>
-      <c r="B522" s="1"/>
-    </row>
-    <row r="529" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A529" s="1"/>
-    </row>
-    <row r="534" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A534" s="1"/>
-      <c r="B534" s="1"/>
-    </row>
-    <row r="541" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A541" s="1"/>
-    </row>
-    <row r="551" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A551" s="1"/>
-      <c r="B551" s="1"/>
-    </row>
-    <row r="558" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A558" s="1"/>
-    </row>
-    <row r="569" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A569" s="1"/>
-      <c r="B569" s="1"/>
-    </row>
-    <row r="576" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A576" s="1"/>
-    </row>
-    <row r="592" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A592" s="1"/>
-      <c r="B592" s="1"/>
-    </row>
-    <row r="599" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A599" s="1"/>
-    </row>
-    <row r="611" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A611" s="1"/>
-      <c r="B611" s="1"/>
-    </row>
-    <row r="618" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A618" s="1"/>
-    </row>
-    <row r="626" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A626" s="1"/>
-      <c r="B626" s="1"/>
+      <c r="B342" s="2"/>
+    </row>
+    <row r="346" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A346" s="1"/>
+    </row>
+    <row r="348" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A348" s="2"/>
+      <c r="G348" s="2"/>
+    </row>
+    <row r="357" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A357" s="1"/>
+      <c r="B357" s="1"/>
+    </row>
+    <row r="364" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A364" s="1"/>
+    </row>
+    <row r="375" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A375" s="1"/>
+      <c r="B375" s="1"/>
+    </row>
+    <row r="382" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A382" s="1"/>
+    </row>
+    <row r="393" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A393" s="1"/>
+      <c r="B393" s="1"/>
+    </row>
+    <row r="400" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A400" s="1"/>
+    </row>
+    <row r="412" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A412" s="1"/>
+      <c r="B412" s="1"/>
+    </row>
+    <row r="419" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A419" s="1"/>
+    </row>
+    <row r="434" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A434" s="1"/>
+      <c r="B434" s="1"/>
+    </row>
+    <row r="441" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A441" s="1"/>
+    </row>
+    <row r="446" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A446" s="1"/>
+      <c r="B446" s="1"/>
+    </row>
+    <row r="453" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A453" s="1"/>
+    </row>
+    <row r="461" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A461" s="1"/>
+      <c r="B461" s="1"/>
+    </row>
+    <row r="468" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A468" s="1"/>
+    </row>
+    <row r="477" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A477" s="1"/>
+      <c r="B477" s="1"/>
+    </row>
+    <row r="484" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A484" s="1"/>
+    </row>
+    <row r="491" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A491" s="1"/>
+      <c r="B491" s="1"/>
+    </row>
+    <row r="498" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A498" s="1"/>
+    </row>
+    <row r="511" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A511" s="1"/>
+      <c r="B511" s="1"/>
+    </row>
+    <row r="518" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A518" s="1"/>
+    </row>
+    <row r="528" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A528" s="1"/>
+      <c r="B528" s="1"/>
+    </row>
+    <row r="535" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A535" s="1"/>
+    </row>
+    <row r="540" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A540" s="1"/>
+      <c r="B540" s="1"/>
+    </row>
+    <row r="547" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A547" s="1"/>
+    </row>
+    <row r="557" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A557" s="1"/>
+      <c r="B557" s="1"/>
+    </row>
+    <row r="564" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A564" s="1"/>
+    </row>
+    <row r="575" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A575" s="1"/>
+      <c r="B575" s="1"/>
+    </row>
+    <row r="582" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A582" s="1"/>
+    </row>
+    <row r="598" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A598" s="1"/>
+      <c r="B598" s="1"/>
+    </row>
+    <row r="605" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A605" s="1"/>
+    </row>
+    <row r="617" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A617" s="1"/>
+      <c r="B617" s="1"/>
+    </row>
+    <row r="624" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A624" s="1"/>
     </row>
     <row r="632" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A632" s="1"/>
+      <c r="B632" s="1"/>
     </row>
     <row r="638" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A638" s="1"/>
-      <c r="B638" s="1"/>
-    </row>
-    <row r="644" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="644" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A644" s="1"/>
-    </row>
-    <row r="664" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A664" s="1"/>
-      <c r="B664" s="1"/>
+      <c r="B644" s="1"/>
+    </row>
+    <row r="650" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A650" s="1"/>
     </row>
     <row r="670" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A670" s="1"/>
+      <c r="B670" s="1"/>
+    </row>
+    <row r="676" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A676" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H670" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H676" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix NG SMR inventories Update wrt Master
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treyer_k\Documents\PSI\elegancy\premise input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8180BA6E-73EE-4578-BC96-61F405B21604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A28196-5628-4A1C-B4A1-ABFD6DDDAED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrogen" sheetId="1" r:id="rId1"/>
@@ -750,7 +750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I678"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1804,7 +1806,7 @@
         <v>33</v>
       </c>
       <c r="B60">
-        <v>1.9949446142967199E-8</v>
+        <v>2.803301033677894E-8</v>
       </c>
       <c r="C60" t="s">
         <v>26</v>
@@ -1830,7 +1832,7 @@
         <v>35</v>
       </c>
       <c r="B61">
-        <v>2.9924169214450796E-6</v>
+        <v>4.2049515505168402E-6</v>
       </c>
       <c r="C61" t="s">
         <v>26</v>
@@ -1856,7 +1858,7 @@
         <v>36</v>
       </c>
       <c r="B62">
-        <v>7.9799679826110004E-6</v>
+        <v>1.1213470456299422E-5</v>
       </c>
       <c r="C62" t="s">
         <v>26</v>
@@ -1882,7 +1884,7 @@
         <v>37</v>
       </c>
       <c r="B63">
-        <v>1.9949446142967197E-10</v>
+        <v>2.8033010336778933E-10</v>
       </c>
       <c r="C63" t="s">
         <v>26</v>
@@ -1908,7 +1910,7 @@
         <v>38</v>
       </c>
       <c r="B64">
-        <v>1.3964991350925282E-5</v>
+        <v>1.9623639878920949E-5</v>
       </c>
       <c r="C64" t="s">
         <v>26</v>
@@ -1934,7 +1936,7 @@
         <v>27</v>
       </c>
       <c r="B65">
-        <v>3.5739278053752441</v>
+        <v>2.6104586734695769</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
@@ -1960,7 +1962,7 @@
         <v>39</v>
       </c>
       <c r="B66">
-        <v>4.18945950019276E-5</v>
+        <v>5.8870386993587143E-5</v>
       </c>
       <c r="C66" t="s">
         <v>26</v>
@@ -1986,7 +1988,7 @@
         <v>40</v>
       </c>
       <c r="B67">
-        <v>1.9949446142967199E-6</v>
+        <v>2.8033010336778938E-6</v>
       </c>
       <c r="C67" t="s">
         <v>26</v>
@@ -2012,7 +2014,7 @@
         <v>41</v>
       </c>
       <c r="B68">
-        <v>1.9949446142967199E-6</v>
+        <v>2.8033010336778938E-6</v>
       </c>
       <c r="C68" t="s">
         <v>26</v>
@@ -2038,7 +2040,7 @@
         <v>42</v>
       </c>
       <c r="B69">
-        <v>5.9850233683142804E-10</v>
+        <v>8.4101694226215283E-10</v>
       </c>
       <c r="C69" t="s">
         <v>26</v>
@@ -2064,7 +2066,7 @@
         <v>43</v>
       </c>
       <c r="B70">
-        <v>3.9900787540175611E-5</v>
+        <v>5.6068683889436346E-5</v>
       </c>
       <c r="C70" t="s">
         <v>26</v>
@@ -2090,7 +2092,7 @@
         <v>44</v>
       </c>
       <c r="B71">
-        <v>3.5710380412862236E-4</v>
+        <v>5.0180313582138397E-4</v>
       </c>
       <c r="C71" t="s">
         <v>26</v>
@@ -2116,7 +2118,7 @@
         <v>45</v>
       </c>
       <c r="B72">
-        <v>1.9949446142967197E-7</v>
+        <v>2.8033010336778935E-7</v>
       </c>
       <c r="C72" t="s">
         <v>26</v>
@@ -2142,7 +2144,7 @@
         <v>46</v>
       </c>
       <c r="B73">
-        <v>3.9900787540175598E-6</v>
+        <v>5.6068683889436342E-6</v>
       </c>
       <c r="C73" t="s">
         <v>26</v>
@@ -2168,7 +2170,7 @@
         <v>47</v>
       </c>
       <c r="B74">
-        <v>2.3940851574953607E-5</v>
+        <v>3.3641742976837502E-5</v>
       </c>
       <c r="C74" t="s">
         <v>26</v>
@@ -2194,7 +2196,7 @@
         <v>48</v>
       </c>
       <c r="B75">
-        <v>3.9900787540175598E-6</v>
+        <v>5.6068683889436342E-6</v>
       </c>
       <c r="C75" t="s">
         <v>26</v>
@@ -2220,7 +2222,7 @@
         <v>49</v>
       </c>
       <c r="B76">
-        <v>3.9900787540175603E-7</v>
+        <v>5.6068683889436334E-7</v>
       </c>
       <c r="C76" t="s">
         <v>26</v>
@@ -2246,7 +2248,7 @@
         <v>50</v>
       </c>
       <c r="B77">
-        <v>1.0972574429480202E-5</v>
+        <v>1.5418688328404109E-5</v>
       </c>
       <c r="C77" t="s">
         <v>26</v>
@@ -2272,7 +2274,7 @@
         <v>51</v>
       </c>
       <c r="B78">
-        <v>3.9900787540175598E-6</v>
+        <v>5.6068683889436342E-6</v>
       </c>
       <c r="C78" t="s">
         <v>26</v>
@@ -2361,7 +2363,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>5.2412402057638054</v>
+        <v>6.1611670196058146</v>
       </c>
       <c r="C82" t="s">
         <v>32</v>
@@ -2479,7 +2481,7 @@
         <v>77</v>
       </c>
       <c r="B87">
-        <v>1.7820216699596938E-4</v>
+        <v>2.0947967866659771E-4</v>
       </c>
       <c r="C87" t="s">
         <v>32</v>
@@ -2663,7 +2665,7 @@
         <v>24</v>
       </c>
       <c r="B95">
-        <v>4.430822860844585</v>
+        <v>4.4303152102137977</v>
       </c>
       <c r="C95" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Fix NG SMR inventories
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-natgas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treyer_k\Documents\PSI\elegancy\premise input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8180BA6E-73EE-4578-BC96-61F405B21604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A28196-5628-4A1C-B4A1-ABFD6DDDAED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrogen" sheetId="1" r:id="rId1"/>
@@ -750,7 +750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I678"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1804,7 +1806,7 @@
         <v>33</v>
       </c>
       <c r="B60">
-        <v>1.9949446142967199E-8</v>
+        <v>2.803301033677894E-8</v>
       </c>
       <c r="C60" t="s">
         <v>26</v>
@@ -1830,7 +1832,7 @@
         <v>35</v>
       </c>
       <c r="B61">
-        <v>2.9924169214450796E-6</v>
+        <v>4.2049515505168402E-6</v>
       </c>
       <c r="C61" t="s">
         <v>26</v>
@@ -1856,7 +1858,7 @@
         <v>36</v>
       </c>
       <c r="B62">
-        <v>7.9799679826110004E-6</v>
+        <v>1.1213470456299422E-5</v>
       </c>
       <c r="C62" t="s">
         <v>26</v>
@@ -1882,7 +1884,7 @@
         <v>37</v>
       </c>
       <c r="B63">
-        <v>1.9949446142967197E-10</v>
+        <v>2.8033010336778933E-10</v>
       </c>
       <c r="C63" t="s">
         <v>26</v>
@@ -1908,7 +1910,7 @@
         <v>38</v>
       </c>
       <c r="B64">
-        <v>1.3964991350925282E-5</v>
+        <v>1.9623639878920949E-5</v>
       </c>
       <c r="C64" t="s">
         <v>26</v>
@@ -1934,7 +1936,7 @@
         <v>27</v>
       </c>
       <c r="B65">
-        <v>3.5739278053752441</v>
+        <v>2.6104586734695769</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
@@ -1960,7 +1962,7 @@
         <v>39</v>
       </c>
       <c r="B66">
-        <v>4.18945950019276E-5</v>
+        <v>5.8870386993587143E-5</v>
       </c>
       <c r="C66" t="s">
         <v>26</v>
@@ -1986,7 +1988,7 @@
         <v>40</v>
       </c>
       <c r="B67">
-        <v>1.9949446142967199E-6</v>
+        <v>2.8033010336778938E-6</v>
       </c>
       <c r="C67" t="s">
         <v>26</v>
@@ -2012,7 +2014,7 @@
         <v>41</v>
       </c>
       <c r="B68">
-        <v>1.9949446142967199E-6</v>
+        <v>2.8033010336778938E-6</v>
       </c>
       <c r="C68" t="s">
         <v>26</v>
@@ -2038,7 +2040,7 @@
         <v>42</v>
       </c>
       <c r="B69">
-        <v>5.9850233683142804E-10</v>
+        <v>8.4101694226215283E-10</v>
       </c>
       <c r="C69" t="s">
         <v>26</v>
@@ -2064,7 +2066,7 @@
         <v>43</v>
       </c>
       <c r="B70">
-        <v>3.9900787540175611E-5</v>
+        <v>5.6068683889436346E-5</v>
       </c>
       <c r="C70" t="s">
         <v>26</v>
@@ -2090,7 +2092,7 @@
         <v>44</v>
       </c>
       <c r="B71">
-        <v>3.5710380412862236E-4</v>
+        <v>5.0180313582138397E-4</v>
       </c>
       <c r="C71" t="s">
         <v>26</v>
@@ -2116,7 +2118,7 @@
         <v>45</v>
       </c>
       <c r="B72">
-        <v>1.9949446142967197E-7</v>
+        <v>2.8033010336778935E-7</v>
       </c>
       <c r="C72" t="s">
         <v>26</v>
@@ -2142,7 +2144,7 @@
         <v>46</v>
       </c>
       <c r="B73">
-        <v>3.9900787540175598E-6</v>
+        <v>5.6068683889436342E-6</v>
       </c>
       <c r="C73" t="s">
         <v>26</v>
@@ -2168,7 +2170,7 @@
         <v>47</v>
       </c>
       <c r="B74">
-        <v>2.3940851574953607E-5</v>
+        <v>3.3641742976837502E-5</v>
       </c>
       <c r="C74" t="s">
         <v>26</v>
@@ -2194,7 +2196,7 @@
         <v>48</v>
       </c>
       <c r="B75">
-        <v>3.9900787540175598E-6</v>
+        <v>5.6068683889436342E-6</v>
       </c>
       <c r="C75" t="s">
         <v>26</v>
@@ -2220,7 +2222,7 @@
         <v>49</v>
       </c>
       <c r="B76">
-        <v>3.9900787540175603E-7</v>
+        <v>5.6068683889436334E-7</v>
       </c>
       <c r="C76" t="s">
         <v>26</v>
@@ -2246,7 +2248,7 @@
         <v>50</v>
       </c>
       <c r="B77">
-        <v>1.0972574429480202E-5</v>
+        <v>1.5418688328404109E-5</v>
       </c>
       <c r="C77" t="s">
         <v>26</v>
@@ -2272,7 +2274,7 @@
         <v>51</v>
       </c>
       <c r="B78">
-        <v>3.9900787540175598E-6</v>
+        <v>5.6068683889436342E-6</v>
       </c>
       <c r="C78" t="s">
         <v>26</v>
@@ -2361,7 +2363,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>5.2412402057638054</v>
+        <v>6.1611670196058146</v>
       </c>
       <c r="C82" t="s">
         <v>32</v>
@@ -2479,7 +2481,7 @@
         <v>77</v>
       </c>
       <c r="B87">
-        <v>1.7820216699596938E-4</v>
+        <v>2.0947967866659771E-4</v>
       </c>
       <c r="C87" t="s">
         <v>32</v>
@@ -2663,7 +2665,7 @@
         <v>24</v>
       </c>
       <c r="B95">
-        <v>4.430822860844585</v>
+        <v>4.4303152102137977</v>
       </c>
       <c r="C95" t="s">
         <v>32</v>

</xml_diff>